<commit_message>
Update APP - Casos de prueba.xlsx
</commit_message>
<xml_diff>
--- a/Documentacion/APP - Casos de prueba.xlsx
+++ b/Documentacion/APP - Casos de prueba.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FACU\ISPC\2024\BankArg-APP-2024\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC90170E-91AB-4A12-8151-BDB98B2A39C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C14C88F-79AB-4EDA-B1C5-70FFFEA3D419}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="49">
   <si>
     <t xml:space="preserve">Proyecto:  </t>
   </si>
@@ -139,12 +139,6 @@
     <t>Nombre de usuario válido</t>
   </si>
   <si>
-    <t>Acceder al perfil del usuario</t>
-  </si>
-  <si>
-    <t>Se ingresa al perfil del usuario perfectamente</t>
-  </si>
-  <si>
     <t>Ingresar Usuario</t>
   </si>
   <si>
@@ -161,6 +155,18 @@
   </si>
   <si>
     <t>Prueba de legibilidad</t>
+  </si>
+  <si>
+    <t>Acceder a la página de inicio</t>
+  </si>
+  <si>
+    <t>Se ingresa al perfil del usuario</t>
+  </si>
+  <si>
+    <t>Reworks 2</t>
+  </si>
+  <si>
+    <t>Al loguearse se debería redirigir al home y no al perfil del usuario</t>
   </si>
 </sst>
 </file>
@@ -170,7 +176,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/mm/yyyy"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -224,6 +230,26 @@
       <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -382,7 +408,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -410,16 +436,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -428,23 +447,44 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -693,12 +733,12 @@
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
       <c r="G2" s="10"/>
       <c r="J2" s="3"/>
     </row>
@@ -723,12 +763,12 @@
       <c r="J4" s="3"/>
     </row>
     <row r="5" spans="1:11" ht="15.75" customHeight="1">
-      <c r="H5" s="21" t="s">
+      <c r="H5" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="31"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1">
       <c r="A6" s="7" t="s">
@@ -766,13 +806,13 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="12.75">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="23">
+      <c r="C7" s="20">
         <v>1</v>
       </c>
       <c r="D7" s="11" t="s">
@@ -781,46 +821,46 @@
       <c r="E7" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="24"/>
-      <c r="G7" s="26" t="s">
+      <c r="F7" s="21"/>
+      <c r="G7" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="29" t="s">
+      <c r="H7" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="I7" s="30" t="s">
+      <c r="I7" s="27" t="s">
         <v>21</v>
       </c>
       <c r="J7" s="16">
         <v>45439</v>
       </c>
-      <c r="K7" s="18"/>
+      <c r="K7" s="19"/>
     </row>
     <row r="8" spans="1:11" ht="38.25">
-      <c r="A8" s="17"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
+      <c r="A8" s="18"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
       <c r="D8" s="11" t="s">
         <v>22</v>
       </c>
       <c r="E8" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="25"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
     </row>
     <row r="9" spans="1:11" ht="12.75">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="C9" s="23">
+      <c r="B9" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="20">
         <v>2</v>
       </c>
       <c r="D9" s="11" t="s">
@@ -829,48 +869,48 @@
       <c r="E9" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="24"/>
-      <c r="G9" s="28" t="s">
+      <c r="F9" s="21"/>
+      <c r="G9" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="H9" s="29" t="s">
+      <c r="H9" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="I9" s="32" t="s">
-        <v>27</v>
+      <c r="I9" s="29" t="s">
+        <v>47</v>
       </c>
       <c r="J9" s="16">
-        <v>45443</v>
-      </c>
-      <c r="K9" s="29" t="s">
-        <v>45</v>
+        <v>45415</v>
+      </c>
+      <c r="K9" s="26" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="63.75">
-      <c r="A10" s="17"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
+      <c r="A10" s="18"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
       <c r="D10" s="11" t="s">
         <v>28</v>
       </c>
       <c r="E10" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="25"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="17"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
     </row>
     <row r="11" spans="1:11" ht="12.75">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="23">
+      <c r="C11" s="20">
         <v>3</v>
       </c>
       <c r="D11" s="11" t="s">
@@ -879,117 +919,119 @@
       <c r="E11" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="24"/>
-      <c r="G11" s="28" t="s">
+      <c r="F11" s="21"/>
+      <c r="G11" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="H11" s="29" t="s">
+      <c r="H11" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="I11" s="30" t="s">
+      <c r="I11" s="27" t="s">
         <v>21</v>
       </c>
       <c r="J11" s="16">
         <v>45444</v>
       </c>
-      <c r="K11" s="18"/>
+      <c r="K11" s="19"/>
     </row>
     <row r="12" spans="1:11" ht="51">
-      <c r="A12" s="17"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
+      <c r="A12" s="18"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
       <c r="D12" s="11" t="s">
         <v>33</v>
       </c>
       <c r="E12" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="25"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="17"/>
-      <c r="K12" s="17"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18"/>
     </row>
     <row r="13" spans="1:11" ht="25.5">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="23">
+      <c r="C13" s="20">
         <v>1</v>
       </c>
       <c r="D13" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="24" t="s">
+      <c r="E13" s="21" t="s">
         <v>37</v>
       </c>
       <c r="F13" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="G13" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="H13" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="I13" s="30" t="s">
-        <v>21</v>
+      <c r="G13" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="H13" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="I13" s="34" t="s">
+        <v>27</v>
       </c>
       <c r="J13" s="16">
         <v>45439</v>
       </c>
-      <c r="K13" s="18"/>
+      <c r="K13" s="37" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="14" spans="1:11" ht="12.75">
-      <c r="A14" s="31"/>
-      <c r="B14" s="31"/>
-      <c r="C14" s="31"/>
+      <c r="A14" s="17"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
       <c r="D14" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="22"/>
+      <c r="F14" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" s="24"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="35"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="38"/>
+    </row>
+    <row r="15" spans="1:11" ht="12.75">
+      <c r="A15" s="17"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="E14" s="25"/>
-      <c r="F14" s="14" t="s">
+      <c r="E15" s="22"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="35"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="38"/>
+    </row>
+    <row r="16" spans="1:11" ht="12.75">
+      <c r="A16" s="18"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="G14" s="33"/>
-      <c r="H14" s="31"/>
-      <c r="I14" s="31"/>
-      <c r="J14" s="31"/>
-      <c r="K14" s="31"/>
-    </row>
-    <row r="15" spans="1:11" ht="12.75">
-      <c r="A15" s="31"/>
-      <c r="B15" s="31"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="E15" s="25"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="31"/>
-      <c r="I15" s="31"/>
-      <c r="J15" s="31"/>
-      <c r="K15" s="31"/>
-    </row>
-    <row r="16" spans="1:11" ht="12.75">
-      <c r="A16" s="17"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="E16" s="25"/>
+      <c r="E16" s="22"/>
       <c r="F16" s="14"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="17"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="36"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="39"/>
     </row>
     <row r="17" spans="10:10" ht="12.75">
       <c r="J17" s="3"/>
@@ -3918,14 +3960,20 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="J13:J16"/>
-    <mergeCell ref="K13:K16"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="C13:C16"/>
-    <mergeCell ref="E13:E16"/>
-    <mergeCell ref="G13:G16"/>
-    <mergeCell ref="H13:H16"/>
-    <mergeCell ref="I13:I16"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="H5:K5"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
     <mergeCell ref="A13:A16"/>
     <mergeCell ref="J9:J10"/>
     <mergeCell ref="K9:K10"/>
@@ -3942,20 +3990,14 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="F11:F12"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="H5:K5"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="J13:J16"/>
+    <mergeCell ref="K13:K16"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="C13:C16"/>
+    <mergeCell ref="E13:E16"/>
+    <mergeCell ref="G13:G16"/>
+    <mergeCell ref="H13:H16"/>
+    <mergeCell ref="I13:I16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>